<commit_message>
New Version of Project Schedule and First version of Master Test Plan
</commit_message>
<xml_diff>
--- a/management/Project Schedule.xlsx
+++ b/management/Project Schedule.xlsx
@@ -1415,6 +1415,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1422,36 +1449,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1852,7 +1852,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2231,7 +2231,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2259,27 +2259,27 @@
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="I1" s="72"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
@@ -2322,11 +2322,11 @@
       <c r="B4" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="79">
+      <c r="C4" s="85">
         <v>43189</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="53"/>
       <c r="G4" s="56" t="s">
         <v>10</v>
@@ -2336,97 +2336,97 @@
       </c>
       <c r="I4" s="54"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="76" t="str">
+      <c r="K4" s="77" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="76" t="str">
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="77" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="76" t="str">
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="77" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="76" t="str">
+      <c r="Z4" s="78"/>
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="77" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="77"/>
-      <c r="AK4" s="77"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="76" t="str">
+      <c r="AG4" s="78"/>
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="78"/>
+      <c r="AK4" s="78"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="77" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="77"/>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="77"/>
-      <c r="AQ4" s="77"/>
-      <c r="AR4" s="77"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="76" t="str">
+      <c r="AN4" s="78"/>
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="77" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="77"/>
-      <c r="AV4" s="77"/>
-      <c r="AW4" s="77"/>
-      <c r="AX4" s="77"/>
-      <c r="AY4" s="77"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="76" t="str">
+      <c r="AU4" s="78"/>
+      <c r="AV4" s="78"/>
+      <c r="AW4" s="78"/>
+      <c r="AX4" s="78"/>
+      <c r="AY4" s="78"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="77" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="77"/>
-      <c r="BC4" s="77"/>
-      <c r="BD4" s="77"/>
-      <c r="BE4" s="77"/>
-      <c r="BF4" s="77"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="76" t="str">
+      <c r="BB4" s="78"/>
+      <c r="BC4" s="78"/>
+      <c r="BD4" s="78"/>
+      <c r="BE4" s="78"/>
+      <c r="BF4" s="78"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="77" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="77"/>
-      <c r="BJ4" s="77"/>
-      <c r="BK4" s="77"/>
-      <c r="BL4" s="77"/>
-      <c r="BM4" s="77"/>
-      <c r="BN4" s="78"/>
+      <c r="BI4" s="78"/>
+      <c r="BJ4" s="78"/>
+      <c r="BK4" s="78"/>
+      <c r="BL4" s="78"/>
+      <c r="BM4" s="78"/>
+      <c r="BN4" s="79"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52"/>
       <c r="B5" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
@@ -3105,7 +3105,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="30">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I9" s="31">
         <f t="shared" si="4"/>
@@ -3178,20 +3178,22 @@
         <v>17</v>
       </c>
       <c r="D10" s="69"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47" t="str">
+      <c r="E10" s="46">
+        <v>43193</v>
+      </c>
+      <c r="F10" s="47">
         <f t="shared" ref="F10" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G10" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="30">
-        <v>0</v>
-      </c>
-      <c r="I10" s="31" t="str">
+        <v>0.7</v>
+      </c>
+      <c r="I10" s="31">
         <f t="shared" ref="I10" si="7">IF(OR(F10=0,E10=0)," - ",NETWORKDAYS(E10,F10))</f>
-        <v xml:space="preserve"> - </v>
+        <v>3</v>
       </c>
       <c r="J10" s="44"/>
       <c r="K10" s="50"/>
@@ -3260,20 +3262,22 @@
         <v>19</v>
       </c>
       <c r="D11" s="69"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47" t="str">
+      <c r="E11" s="46">
+        <v>43193</v>
+      </c>
+      <c r="F11" s="47">
         <f t="shared" ref="F11" si="8">IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G11" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="30">
-        <v>0</v>
-      </c>
-      <c r="I11" s="31" t="str">
+        <v>0.8</v>
+      </c>
+      <c r="I11" s="31">
         <f t="shared" ref="I11" si="9">IF(OR(F11=0,E11=0)," - ",NETWORKDAYS(E11,F11))</f>
-        <v xml:space="preserve"> - </v>
+        <v>3</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="50"/>
@@ -3353,7 +3357,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="30">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I12" s="31">
         <f t="shared" ref="I12" si="10">IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
@@ -3430,14 +3434,14 @@
         <v>43189</v>
       </c>
       <c r="F13" s="47">
-        <f t="shared" ref="F13:F23" si="11">IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+        <f t="shared" ref="E13:F24" si="11">IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
         <v>43193</v>
       </c>
       <c r="G13" s="29">
         <v>5</v>
       </c>
       <c r="H13" s="30">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I13" s="31">
         <f t="shared" si="4"/>
@@ -3506,7 +3510,7 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.1</v>
       </c>
-      <c r="B14" s="83" t="s">
+      <c r="B14" s="74" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="69"/>
@@ -3590,24 +3594,26 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.2</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="75" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="69"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47" t="str">
+      <c r="E15" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F15" s="47">
         <f t="shared" ref="F15" si="14">IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G15" s="29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H15" s="30">
-        <v>0</v>
-      </c>
-      <c r="I15" s="31" t="str">
+        <v>0.8</v>
+      </c>
+      <c r="I15" s="31">
         <f t="shared" ref="I15" si="15">IF(OR(F15=0,E15=0)," - ",NETWORKDAYS(E15,F15))</f>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="J15" s="44"/>
       <c r="K15" s="50"/>
@@ -3672,24 +3678,26 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.3</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="75" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="69"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47" t="str">
+      <c r="E16" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F16" s="47">
         <f t="shared" ref="F16" si="16">IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G16" s="29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H16" s="30">
-        <v>0</v>
-      </c>
-      <c r="I16" s="31" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="I16" s="31">
         <f t="shared" ref="I16" si="17">IF(OR(F16=0,E16=0)," - ",NETWORKDAYS(E16,F16))</f>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="J16" s="44"/>
       <c r="K16" s="50"/>
@@ -3754,24 +3762,26 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.4</v>
       </c>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="74" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="69"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47" t="str">
+      <c r="E17" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F17" s="47">
         <f t="shared" ref="F17" si="18">IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G17" s="29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H17" s="30">
-        <v>0</v>
-      </c>
-      <c r="I17" s="31" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="I17" s="31">
         <f t="shared" ref="I17" si="19">IF(OR(F17=0,E17=0)," - ",NETWORKDAYS(E17,F17))</f>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="J17" s="44"/>
       <c r="K17" s="50"/>
@@ -3836,24 +3846,26 @@
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.5</v>
       </c>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="76" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="69"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47" t="str">
+      <c r="E18" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F18" s="47">
         <f t="shared" ref="F18" si="20">IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G18" s="29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H18" s="30">
-        <v>0</v>
-      </c>
-      <c r="I18" s="31" t="str">
+        <v>0.9</v>
+      </c>
+      <c r="I18" s="31">
         <f t="shared" ref="I18" si="21">IF(OR(F18=0,E18=0)," - ",NETWORKDAYS(E18,F18))</f>
-        <v xml:space="preserve"> - </v>
+        <v>5</v>
       </c>
       <c r="J18" s="44"/>
       <c r="K18" s="50"/>
@@ -4172,20 +4184,21 @@
         <v>27</v>
       </c>
       <c r="D22" s="69"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47" t="str">
+      <c r="E22" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F22" s="47">
         <f t="shared" si="11"/>
-        <v xml:space="preserve"> - </v>
+        <v>43193</v>
       </c>
       <c r="G22" s="29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="30">
-        <v>0</v>
-      </c>
-      <c r="I22" s="31" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
+        <v>1</v>
+      </c>
+      <c r="I22" s="31">
+        <v>3</v>
       </c>
       <c r="J22" s="44"/>
       <c r="K22" s="50"/>
@@ -4254,20 +4267,21 @@
         <v>30</v>
       </c>
       <c r="D23" s="69"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="47" t="str">
+      <c r="E23" s="46">
+        <v>43189</v>
+      </c>
+      <c r="F23" s="47">
         <f t="shared" si="11"/>
-        <v xml:space="preserve"> - </v>
+        <v>43195</v>
       </c>
       <c r="G23" s="29">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H23" s="30">
         <v>0</v>
       </c>
-      <c r="I23" s="31" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
+      <c r="I23" s="31">
+        <v>5</v>
       </c>
       <c r="J23" s="44"/>
       <c r="K23" s="50"/>
@@ -4336,20 +4350,22 @@
         <v>31</v>
       </c>
       <c r="D24" s="69"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47" t="str">
+      <c r="E24" s="46">
+        <v>43193</v>
+      </c>
+      <c r="F24" s="47">
         <f t="shared" ref="F24" si="22">IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
-        <v xml:space="preserve"> - </v>
+        <v>43196</v>
       </c>
       <c r="G24" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H24" s="30">
         <v>0</v>
       </c>
-      <c r="I24" s="31" t="str">
+      <c r="I24" s="31">
         <f t="shared" ref="I24" si="23">IF(OR(F24=0,E24=0)," - ",NETWORKDAYS(E24,F24))</f>
-        <v xml:space="preserve"> - </v>
+        <v>4</v>
       </c>
       <c r="J24" s="44"/>
       <c r="K24" s="50"/>
@@ -4480,6 +4496,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -4490,15 +4515,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H9 H13 H19:H20 H22:H23">
@@ -4778,7 +4794,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="G13 H19 H23" unlockedFormula="1"/>
+    <ignoredError sqref="G13 H19" unlockedFormula="1"/>
     <ignoredError sqref="A19" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update reviewers for the designs in project Schedule
</commit_message>
<xml_diff>
--- a/management/Project Schedule.xlsx
+++ b/management/Project Schedule.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="13275" windowHeight="11250"/>
@@ -18,7 +18,7 @@
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>WBS</t>
   </si>
@@ -559,25 +559,10 @@
     <t>Operating System</t>
   </si>
   <si>
-    <t>Abdel Rahman , El Zeiny</t>
-  </si>
-  <si>
     <t xml:space="preserve">Raafat , Basma </t>
   </si>
   <si>
     <t>Raafat,Basma , Esraa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raafat , Christine </t>
-  </si>
-  <si>
-    <t>Raafat , El Zeiny</t>
-  </si>
-  <si>
-    <t>Khaled , Christine</t>
-  </si>
-  <si>
-    <t>Abdel Rahman , Khaled</t>
   </si>
   <si>
     <t>N/A</t>
@@ -676,18 +661,39 @@
     <t>Button 
 BugFixing</t>
   </si>
+  <si>
+    <t xml:space="preserve">Abdel Rahman </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khaled </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raafat </t>
+  </si>
+  <si>
+    <t>Abdel Rahman</t>
+  </si>
+  <si>
+    <t>Raafat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ \(dddd\)"/>
     <numFmt numFmtId="165" formatCode="ddd\ m/dd/yy"/>
     <numFmt numFmtId="166" formatCode="d"/>
     <numFmt numFmtId="167" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1575,6 +1581,19 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1584,6 +1603,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1591,23 +1614,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1657,7 +1663,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="152">
+  <dxfs count="101">
     <dxf>
       <border>
         <left style="thin">
@@ -2399,20 +2405,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2425,20 +2417,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2451,20 +2429,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2477,20 +2441,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2503,6 +2453,20 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2515,6 +2479,20 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2527,6 +2505,20 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -2539,96 +2531,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF0070C0"/>
@@ -2649,344 +2551,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3077,6 +2641,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
@@ -3097,7 +2665,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3131,13 +2699,54 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>28</xdr:col>
+          <xdr:colOff>104775</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8238" name="Scroll Bar 46" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s8238"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3427,18 +3036,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BO60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="G24"/>
+      <pane ySplit="7" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
@@ -3454,7 +3063,7 @@
     <col min="68" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="30" customHeight="1">
+    <row r="1" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
         <v>11</v>
       </c>
@@ -3465,29 +3074,29 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="67"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="73"/>
+      <c r="AC1" s="73"/>
+      <c r="AD1" s="73"/>
+      <c r="AE1" s="73"/>
+      <c r="AF1" s="73"/>
     </row>
-    <row r="2" spans="1:67" ht="18" customHeight="1">
+    <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3497,7 +3106,7 @@
       <c r="G2" s="68"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:67" ht="14.25">
+    <row r="3" spans="1:67" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -3525,17 +3134,17 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
     </row>
-    <row r="4" spans="1:67" ht="17.25" customHeight="1">
+    <row r="4" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="48"/>
       <c r="B4" s="52" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="52"/>
-      <c r="D4" s="79">
+      <c r="D4" s="78">
         <v>43189</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
       <c r="G4" s="49"/>
       <c r="H4" s="52" t="s">
         <v>8</v>
@@ -3545,185 +3154,185 @@
       </c>
       <c r="J4" s="50"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="71" t="str">
+      <c r="L4" s="75" t="str">
         <f>"Week "&amp;(L6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="71" t="str">
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="75" t="str">
         <f>"Week "&amp;(S6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="T4" s="72"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="71" t="str">
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="75" t="str">
         <f>"Week "&amp;(Z6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="71" t="str">
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76"/>
+      <c r="AF4" s="77"/>
+      <c r="AG4" s="75" t="str">
         <f>"Week "&amp;(AG6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="72"/>
-      <c r="AL4" s="72"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="71" t="str">
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="77"/>
+      <c r="AN4" s="75" t="str">
         <f>"Week "&amp;(AN6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="71" t="str">
+      <c r="AO4" s="76"/>
+      <c r="AP4" s="76"/>
+      <c r="AQ4" s="76"/>
+      <c r="AR4" s="76"/>
+      <c r="AS4" s="76"/>
+      <c r="AT4" s="77"/>
+      <c r="AU4" s="75" t="str">
         <f>"Week "&amp;(AU6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AV4" s="72"/>
-      <c r="AW4" s="72"/>
-      <c r="AX4" s="72"/>
-      <c r="AY4" s="72"/>
-      <c r="AZ4" s="72"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="71" t="str">
+      <c r="AV4" s="76"/>
+      <c r="AW4" s="76"/>
+      <c r="AX4" s="76"/>
+      <c r="AY4" s="76"/>
+      <c r="AZ4" s="76"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="75" t="str">
         <f>"Week "&amp;(BB6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BC4" s="72"/>
-      <c r="BD4" s="72"/>
-      <c r="BE4" s="72"/>
-      <c r="BF4" s="72"/>
-      <c r="BG4" s="72"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="71" t="str">
+      <c r="BC4" s="76"/>
+      <c r="BD4" s="76"/>
+      <c r="BE4" s="76"/>
+      <c r="BF4" s="76"/>
+      <c r="BG4" s="76"/>
+      <c r="BH4" s="77"/>
+      <c r="BI4" s="75" t="str">
         <f>"Week "&amp;(BI6-($D$4-WEEKDAY($D$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BJ4" s="72"/>
-      <c r="BK4" s="72"/>
-      <c r="BL4" s="72"/>
-      <c r="BM4" s="72"/>
-      <c r="BN4" s="72"/>
-      <c r="BO4" s="73"/>
+      <c r="BJ4" s="76"/>
+      <c r="BK4" s="76"/>
+      <c r="BL4" s="76"/>
+      <c r="BM4" s="76"/>
+      <c r="BN4" s="76"/>
+      <c r="BO4" s="77"/>
     </row>
-    <row r="5" spans="1:67" ht="17.25" customHeight="1">
+    <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48"/>
       <c r="B5" s="52" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="52"/>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
       <c r="G5" s="51"/>
       <c r="H5" s="51"/>
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="74">
+      <c r="L5" s="79">
         <f>L6</f>
         <v>43185</v>
       </c>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="76"/>
-      <c r="S5" s="74">
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="79">
         <f>S6</f>
         <v>43192</v>
       </c>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="76"/>
-      <c r="Z5" s="74">
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="79">
         <f>Z6</f>
         <v>43199</v>
       </c>
-      <c r="AA5" s="75"/>
-      <c r="AB5" s="75"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="75"/>
-      <c r="AF5" s="76"/>
-      <c r="AG5" s="74">
+      <c r="AA5" s="80"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="80"/>
+      <c r="AD5" s="80"/>
+      <c r="AE5" s="80"/>
+      <c r="AF5" s="81"/>
+      <c r="AG5" s="79">
         <f>AG6</f>
         <v>43206</v>
       </c>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="75"/>
-      <c r="AL5" s="75"/>
-      <c r="AM5" s="76"/>
-      <c r="AN5" s="74">
+      <c r="AH5" s="80"/>
+      <c r="AI5" s="80"/>
+      <c r="AJ5" s="80"/>
+      <c r="AK5" s="80"/>
+      <c r="AL5" s="80"/>
+      <c r="AM5" s="81"/>
+      <c r="AN5" s="79">
         <f>AN6</f>
         <v>43213</v>
       </c>
-      <c r="AO5" s="75"/>
-      <c r="AP5" s="75"/>
-      <c r="AQ5" s="75"/>
-      <c r="AR5" s="75"/>
-      <c r="AS5" s="75"/>
-      <c r="AT5" s="76"/>
-      <c r="AU5" s="74">
+      <c r="AO5" s="80"/>
+      <c r="AP5" s="80"/>
+      <c r="AQ5" s="80"/>
+      <c r="AR5" s="80"/>
+      <c r="AS5" s="80"/>
+      <c r="AT5" s="81"/>
+      <c r="AU5" s="79">
         <f>AU6</f>
         <v>43220</v>
       </c>
-      <c r="AV5" s="75"/>
-      <c r="AW5" s="75"/>
-      <c r="AX5" s="75"/>
-      <c r="AY5" s="75"/>
-      <c r="AZ5" s="75"/>
-      <c r="BA5" s="76"/>
-      <c r="BB5" s="74">
+      <c r="AV5" s="80"/>
+      <c r="AW5" s="80"/>
+      <c r="AX5" s="80"/>
+      <c r="AY5" s="80"/>
+      <c r="AZ5" s="80"/>
+      <c r="BA5" s="81"/>
+      <c r="BB5" s="79">
         <f>BB6</f>
         <v>43227</v>
       </c>
-      <c r="BC5" s="75"/>
-      <c r="BD5" s="75"/>
-      <c r="BE5" s="75"/>
-      <c r="BF5" s="75"/>
-      <c r="BG5" s="75"/>
-      <c r="BH5" s="76"/>
-      <c r="BI5" s="74">
+      <c r="BC5" s="80"/>
+      <c r="BD5" s="80"/>
+      <c r="BE5" s="80"/>
+      <c r="BF5" s="80"/>
+      <c r="BG5" s="80"/>
+      <c r="BH5" s="81"/>
+      <c r="BI5" s="79">
         <f>BI6</f>
         <v>43234</v>
       </c>
-      <c r="BJ5" s="75"/>
-      <c r="BK5" s="75"/>
-      <c r="BL5" s="75"/>
-      <c r="BM5" s="75"/>
-      <c r="BN5" s="75"/>
-      <c r="BO5" s="76"/>
+      <c r="BJ5" s="80"/>
+      <c r="BK5" s="80"/>
+      <c r="BL5" s="80"/>
+      <c r="BM5" s="80"/>
+      <c r="BN5" s="80"/>
+      <c r="BO5" s="81"/>
     </row>
-    <row r="6" spans="1:67">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -3960,7 +3569,7 @@
         <v>43240</v>
       </c>
     </row>
-    <row r="7" spans="1:67" s="62" customFormat="1" ht="24.75" thickBot="1">
+    <row r="7" spans="1:67" s="62" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>0</v>
       </c>
@@ -4217,7 +3826,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="8" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -4297,7 +3906,7 @@
       <c r="BN8" s="45"/>
       <c r="BO8" s="45"/>
     </row>
-    <row r="9" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="9" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="str">
         <f t="shared" ref="A9:A13" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -4308,7 +3917,7 @@
       <c r="C9" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="80" t="s">
+      <c r="D9" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E9" s="65"/>
@@ -4387,7 +3996,7 @@
       <c r="BN9" s="46"/>
       <c r="BO9" s="46"/>
     </row>
-    <row r="10" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="10" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
@@ -4398,7 +4007,7 @@
       <c r="C10" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E10" s="65"/>
@@ -4477,7 +4086,7 @@
       <c r="BN10" s="46"/>
       <c r="BO10" s="46"/>
     </row>
-    <row r="11" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="11" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.2</v>
@@ -4488,7 +4097,7 @@
       <c r="C11" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="65"/>
@@ -4567,7 +4176,7 @@
       <c r="BN11" s="46"/>
       <c r="BO11" s="46"/>
     </row>
-    <row r="12" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="12" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.3</v>
@@ -4578,7 +4187,7 @@
       <c r="C12" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="71" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="65"/>
@@ -4657,7 +4266,7 @@
       <c r="BN12" s="46"/>
       <c r="BO12" s="46"/>
     </row>
-    <row r="13" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="13" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="str">
         <f t="shared" si="5"/>
         <v>1.2</v>
@@ -4666,9 +4275,9 @@
         <v>18</v>
       </c>
       <c r="C13" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="71" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="65"/>
@@ -4746,7 +4355,7 @@
       <c r="BN13" s="46"/>
       <c r="BO13" s="46"/>
     </row>
-    <row r="14" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="14" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.1</v>
@@ -4755,10 +4364,10 @@
         <v>21</v>
       </c>
       <c r="C14" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="80" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>62</v>
       </c>
       <c r="E14" s="65"/>
       <c r="F14" s="42">
@@ -4835,7 +4444,7 @@
       <c r="BN14" s="46"/>
       <c r="BO14" s="46"/>
     </row>
-    <row r="15" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="15" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.2</v>
@@ -4846,7 +4455,7 @@
       <c r="C15" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="80" t="s">
+      <c r="D15" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="65"/>
@@ -4925,7 +4534,7 @@
       <c r="BN15" s="46"/>
       <c r="BO15" s="46"/>
     </row>
-    <row r="16" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="16" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.3</v>
@@ -4936,7 +4545,7 @@
       <c r="C16" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="65"/>
@@ -5015,7 +4624,7 @@
       <c r="BN16" s="46"/>
       <c r="BO16" s="46"/>
     </row>
-    <row r="17" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="17" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.4</v>
@@ -5024,9 +4633,9 @@
         <v>20</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="71" t="s">
         <v>32</v>
       </c>
       <c r="E17" s="65"/>
@@ -5104,7 +4713,7 @@
       <c r="BN17" s="46"/>
       <c r="BO17" s="46"/>
     </row>
-    <row r="18" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="18" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.2.5</v>
@@ -5115,7 +4724,7 @@
       <c r="C18" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="80" t="s">
+      <c r="D18" s="71" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="65"/>
@@ -5194,7 +4803,7 @@
       <c r="BN18" s="46"/>
       <c r="BO18" s="46"/>
     </row>
-    <row r="19" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="19" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
@@ -5203,7 +4812,7 @@
         <v>24</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="81"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="19"/>
       <c r="F19" s="42"/>
       <c r="G19" s="44"/>
@@ -5268,7 +4877,7 @@
       <c r="BN19" s="47"/>
       <c r="BO19" s="47"/>
     </row>
-    <row r="20" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="20" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
@@ -5277,9 +4886,9 @@
         <v>26</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="65"/>
@@ -5357,7 +4966,7 @@
       <c r="BN20" s="46"/>
       <c r="BO20" s="46"/>
     </row>
-    <row r="21" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="21" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
@@ -5366,9 +4975,9 @@
         <v>27</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E21" s="65"/>
@@ -5446,7 +5055,7 @@
       <c r="BN21" s="46"/>
       <c r="BO21" s="46"/>
     </row>
-    <row r="22" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="22" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.3</v>
@@ -5455,9 +5064,9 @@
         <v>25</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="71" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="65"/>
@@ -5534,7 +5143,7 @@
       <c r="BN22" s="46"/>
       <c r="BO22" s="46"/>
     </row>
-    <row r="23" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="23" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.4</v>
@@ -5545,7 +5154,7 @@
       <c r="C23" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E23" s="65"/>
@@ -5622,7 +5231,7 @@
       <c r="BN23" s="46"/>
       <c r="BO23" s="46"/>
     </row>
-    <row r="24" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="24" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.5</v>
@@ -5633,7 +5242,7 @@
       <c r="C24" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="80" t="s">
+      <c r="D24" s="71" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="65"/>
@@ -5711,15 +5320,15 @@
       <c r="BN24" s="46"/>
       <c r="BO24" s="46"/>
     </row>
-    <row r="25" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="25" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="16">
         <v>3</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="81"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="19"/>
       <c r="F25" s="42"/>
       <c r="G25" s="44"/>
@@ -5784,7 +5393,7 @@
       <c r="BN25" s="47"/>
       <c r="BO25" s="47"/>
     </row>
-    <row r="26" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="26" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="23">
         <v>3.1</v>
       </c>
@@ -5792,10 +5401,10 @@
         <v>45</v>
       </c>
       <c r="C26" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="80" t="s">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>80</v>
       </c>
       <c r="E26" s="65"/>
       <c r="F26" s="42">
@@ -5808,7 +5417,7 @@
         <v>3</v>
       </c>
       <c r="I26" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="27">
         <v>1</v>
@@ -5871,7 +5480,7 @@
       <c r="BN26" s="46"/>
       <c r="BO26" s="46"/>
     </row>
-    <row r="27" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="27" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="23">
         <v>3.2</v>
       </c>
@@ -5879,10 +5488,10 @@
         <v>44</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="80" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="D27" s="71" t="s">
+        <v>84</v>
       </c>
       <c r="E27" s="65"/>
       <c r="F27" s="42">
@@ -5895,7 +5504,7 @@
         <v>3</v>
       </c>
       <c r="I27" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="27">
         <v>1</v>
@@ -5958,7 +5567,7 @@
       <c r="BN27" s="46"/>
       <c r="BO27" s="46"/>
     </row>
-    <row r="28" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="28" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="23">
         <v>3.3</v>
       </c>
@@ -5966,10 +5575,10 @@
         <v>46</v>
       </c>
       <c r="C28" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="80" t="s">
-        <v>56</v>
+        <v>86</v>
+      </c>
+      <c r="D28" s="71" t="s">
+        <v>42</v>
       </c>
       <c r="E28" s="65"/>
       <c r="F28" s="42">
@@ -5982,7 +5591,7 @@
         <v>7</v>
       </c>
       <c r="I28" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="27">
         <v>5</v>
@@ -6045,7 +5654,7 @@
       <c r="BN28" s="46"/>
       <c r="BO28" s="46"/>
     </row>
-    <row r="29" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="29" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="23">
         <v>3.4</v>
       </c>
@@ -6053,10 +5662,10 @@
         <v>48</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="80" t="s">
-        <v>56</v>
+        <v>81</v>
+      </c>
+      <c r="D29" s="71" t="s">
+        <v>82</v>
       </c>
       <c r="E29" s="65"/>
       <c r="F29" s="42">
@@ -6069,7 +5678,7 @@
         <v>4</v>
       </c>
       <c r="I29" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="27">
         <v>4</v>
@@ -6132,7 +5741,7 @@
       <c r="BN29" s="46"/>
       <c r="BO29" s="46"/>
     </row>
-    <row r="30" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="30" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="23">
         <v>3.5</v>
       </c>
@@ -6140,10 +5749,10 @@
         <v>47</v>
       </c>
       <c r="C30" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="80" t="s">
-        <v>56</v>
+        <v>85</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>34</v>
       </c>
       <c r="E30" s="65"/>
       <c r="F30" s="42">
@@ -6156,7 +5765,7 @@
         <v>4</v>
       </c>
       <c r="I30" s="26">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J30" s="27">
         <v>4</v>
@@ -6219,15 +5828,15 @@
       <c r="BN30" s="46"/>
       <c r="BO30" s="46"/>
     </row>
-    <row r="31" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="31" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="16">
         <v>4</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C31" s="17"/>
-      <c r="D31" s="81"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="19"/>
       <c r="F31" s="42"/>
       <c r="G31" s="44"/>
@@ -6292,16 +5901,16 @@
       <c r="BN31" s="47"/>
       <c r="BO31" s="47"/>
     </row>
-    <row r="32" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="32" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="23">
         <v>4.0999999999999996</v>
       </c>
       <c r="B32" s="64" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C32" s="64"/>
-      <c r="D32" s="80" t="s">
-        <v>56</v>
+      <c r="D32" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E32" s="65"/>
       <c r="F32" s="42">
@@ -6317,7 +5926,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K32" s="40"/>
       <c r="L32" s="46"/>
@@ -6377,16 +5986,16 @@
       <c r="BN32" s="46"/>
       <c r="BO32" s="46"/>
     </row>
-    <row r="33" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="33" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="23">
         <v>4.2</v>
       </c>
       <c r="B33" s="64" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C33" s="64"/>
-      <c r="D33" s="80" t="s">
-        <v>56</v>
+      <c r="D33" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E33" s="65"/>
       <c r="F33" s="42">
@@ -6402,7 +6011,7 @@
         <v>0</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K33" s="40"/>
       <c r="L33" s="46"/>
@@ -6462,16 +6071,16 @@
       <c r="BN33" s="46"/>
       <c r="BO33" s="46"/>
     </row>
-    <row r="34" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="34" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A34" s="23">
         <v>4.3</v>
       </c>
       <c r="B34" s="64" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C34" s="64"/>
-      <c r="D34" s="80" t="s">
-        <v>56</v>
+      <c r="D34" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E34" s="65"/>
       <c r="F34" s="42">
@@ -6487,7 +6096,7 @@
         <v>0</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K34" s="40"/>
       <c r="L34" s="46"/>
@@ -6547,16 +6156,16 @@
       <c r="BN34" s="46"/>
       <c r="BO34" s="46"/>
     </row>
-    <row r="35" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="35" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="23">
         <v>4.4000000000000004</v>
       </c>
       <c r="B35" s="64" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C35" s="64"/>
-      <c r="D35" s="80" t="s">
-        <v>56</v>
+      <c r="D35" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E35" s="65"/>
       <c r="F35" s="42">
@@ -6572,7 +6181,7 @@
         <v>0</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K35" s="40"/>
       <c r="L35" s="46"/>
@@ -6632,16 +6241,16 @@
       <c r="BN35" s="46"/>
       <c r="BO35" s="46"/>
     </row>
-    <row r="36" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="36" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="23">
         <v>4.5</v>
       </c>
       <c r="B36" s="64" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C36" s="64"/>
-      <c r="D36" s="80" t="s">
-        <v>56</v>
+      <c r="D36" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E36" s="65"/>
       <c r="F36" s="42">
@@ -6657,7 +6266,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K36" s="40"/>
       <c r="L36" s="46"/>
@@ -6717,15 +6326,15 @@
       <c r="BN36" s="46"/>
       <c r="BO36" s="46"/>
     </row>
-    <row r="37" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="37" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="16">
         <v>5</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="81"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="19"/>
       <c r="F37" s="42"/>
       <c r="G37" s="44"/>
@@ -6790,16 +6399,16 @@
       <c r="BN37" s="47"/>
       <c r="BO37" s="47"/>
     </row>
-    <row r="38" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="38" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="23">
         <v>5.0999999999999996</v>
       </c>
       <c r="B38" s="64" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C38" s="64"/>
-      <c r="D38" s="80" t="s">
-        <v>56</v>
+      <c r="D38" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E38" s="65"/>
       <c r="F38" s="42">
@@ -6815,7 +6424,7 @@
         <v>0</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K38" s="40"/>
       <c r="L38" s="46"/>
@@ -6875,16 +6484,16 @@
       <c r="BN38" s="46"/>
       <c r="BO38" s="46"/>
     </row>
-    <row r="39" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="39" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="23">
         <v>5.2</v>
       </c>
       <c r="B39" s="64" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C39" s="64"/>
-      <c r="D39" s="80" t="s">
-        <v>56</v>
+      <c r="D39" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E39" s="65"/>
       <c r="F39" s="42">
@@ -6900,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="J39" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K39" s="40"/>
       <c r="L39" s="46"/>
@@ -6960,16 +6569,16 @@
       <c r="BN39" s="46"/>
       <c r="BO39" s="46"/>
     </row>
-    <row r="40" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="40" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A40" s="23">
         <v>5.3</v>
       </c>
       <c r="B40" s="64" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C40" s="64"/>
-      <c r="D40" s="80" t="s">
-        <v>56</v>
+      <c r="D40" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E40" s="65"/>
       <c r="F40" s="42">
@@ -6985,7 +6594,7 @@
         <v>0</v>
       </c>
       <c r="J40" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K40" s="40"/>
       <c r="L40" s="46"/>
@@ -7045,16 +6654,16 @@
       <c r="BN40" s="46"/>
       <c r="BO40" s="46"/>
     </row>
-    <row r="41" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="41" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="23">
         <v>5.4</v>
       </c>
       <c r="B41" s="64" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C41" s="64"/>
-      <c r="D41" s="80" t="s">
-        <v>56</v>
+      <c r="D41" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E41" s="65"/>
       <c r="F41" s="42">
@@ -7070,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="J41" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K41" s="40"/>
       <c r="L41" s="46"/>
@@ -7130,16 +6739,16 @@
       <c r="BN41" s="46"/>
       <c r="BO41" s="46"/>
     </row>
-    <row r="42" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="42" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="23">
         <v>5.5</v>
       </c>
       <c r="B42" s="64" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C42" s="64"/>
-      <c r="D42" s="80" t="s">
-        <v>56</v>
+      <c r="D42" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E42" s="65"/>
       <c r="F42" s="42">
@@ -7155,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="J42" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K42" s="40"/>
       <c r="L42" s="46"/>
@@ -7215,16 +6824,16 @@
       <c r="BN42" s="46"/>
       <c r="BO42" s="46"/>
     </row>
-    <row r="43" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="43" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="23">
         <v>5.6</v>
       </c>
       <c r="B43" s="64" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C43" s="64"/>
-      <c r="D43" s="80" t="s">
-        <v>56</v>
+      <c r="D43" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E43" s="65"/>
       <c r="F43" s="42">
@@ -7240,7 +6849,7 @@
         <v>0</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K43" s="40"/>
       <c r="L43" s="46"/>
@@ -7300,16 +6909,16 @@
       <c r="BN43" s="46"/>
       <c r="BO43" s="46"/>
     </row>
-    <row r="44" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="44" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="23">
         <v>5.7</v>
       </c>
       <c r="B44" s="64" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C44" s="64"/>
-      <c r="D44" s="80" t="s">
-        <v>56</v>
+      <c r="D44" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E44" s="65"/>
       <c r="F44" s="42">
@@ -7325,7 +6934,7 @@
         <v>0</v>
       </c>
       <c r="J44" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K44" s="40"/>
       <c r="L44" s="46"/>
@@ -7385,16 +6994,16 @@
       <c r="BN44" s="46"/>
       <c r="BO44" s="46"/>
     </row>
-    <row r="45" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="45" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="23">
         <v>5.8</v>
       </c>
       <c r="B45" s="64" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C45" s="64"/>
-      <c r="D45" s="80" t="s">
-        <v>56</v>
+      <c r="D45" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E45" s="65"/>
       <c r="F45" s="42">
@@ -7410,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="J45" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K45" s="40"/>
       <c r="L45" s="46"/>
@@ -7470,16 +7079,16 @@
       <c r="BN45" s="46"/>
       <c r="BO45" s="46"/>
     </row>
-    <row r="46" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="46" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="23">
         <v>5.9</v>
       </c>
       <c r="B46" s="64" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C46" s="64"/>
-      <c r="D46" s="80" t="s">
-        <v>56</v>
+      <c r="D46" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E46" s="65"/>
       <c r="F46" s="42">
@@ -7495,7 +7104,7 @@
         <v>0</v>
       </c>
       <c r="J46" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K46" s="40"/>
       <c r="L46" s="46"/>
@@ -7555,16 +7164,16 @@
       <c r="BN46" s="46"/>
       <c r="BO46" s="46"/>
     </row>
-    <row r="47" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="47" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A47" s="23">
         <v>5.0999999999999996</v>
       </c>
       <c r="B47" s="64" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C47" s="64"/>
-      <c r="D47" s="80" t="s">
-        <v>56</v>
+      <c r="D47" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E47" s="65"/>
       <c r="F47" s="42">
@@ -7580,7 +7189,7 @@
         <v>0</v>
       </c>
       <c r="J47" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K47" s="40"/>
       <c r="L47" s="46"/>
@@ -7640,16 +7249,16 @@
       <c r="BN47" s="46"/>
       <c r="BO47" s="46"/>
     </row>
-    <row r="48" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="48" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="23">
         <v>5.1100000000000003</v>
       </c>
       <c r="B48" s="64" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C48" s="64"/>
-      <c r="D48" s="80" t="s">
-        <v>56</v>
+      <c r="D48" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E48" s="65"/>
       <c r="F48" s="42">
@@ -7665,7 +7274,7 @@
         <v>0</v>
       </c>
       <c r="J48" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K48" s="40"/>
       <c r="L48" s="46"/>
@@ -7725,16 +7334,16 @@
       <c r="BN48" s="46"/>
       <c r="BO48" s="46"/>
     </row>
-    <row r="49" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="49" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="23">
         <v>5.12</v>
       </c>
       <c r="B49" s="64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C49" s="64"/>
-      <c r="D49" s="80" t="s">
-        <v>56</v>
+      <c r="D49" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E49" s="65"/>
       <c r="F49" s="42">
@@ -7750,7 +7359,7 @@
         <v>0</v>
       </c>
       <c r="J49" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K49" s="40"/>
       <c r="L49" s="46"/>
@@ -7810,16 +7419,16 @@
       <c r="BN49" s="46"/>
       <c r="BO49" s="46"/>
     </row>
-    <row r="50" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="50" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="23">
         <v>5.13</v>
       </c>
       <c r="B50" s="64" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C50" s="64"/>
-      <c r="D50" s="80" t="s">
-        <v>56</v>
+      <c r="D50" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E50" s="65"/>
       <c r="F50" s="42">
@@ -7835,7 +7444,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K50" s="40"/>
       <c r="L50" s="46"/>
@@ -7895,15 +7504,15 @@
       <c r="BN50" s="46"/>
       <c r="BO50" s="46"/>
     </row>
-    <row r="51" spans="1:67" s="18" customFormat="1" ht="18">
+    <row r="51" spans="1:67" s="18" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="16">
         <v>6</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C51" s="17"/>
-      <c r="D51" s="81"/>
+      <c r="D51" s="72"/>
       <c r="E51" s="19"/>
       <c r="F51" s="42"/>
       <c r="G51" s="44"/>
@@ -7968,16 +7577,16 @@
       <c r="BN51" s="47"/>
       <c r="BO51" s="47"/>
     </row>
-    <row r="52" spans="1:67" s="24" customFormat="1" ht="24">
+    <row r="52" spans="1:67" s="24" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A52" s="23">
         <v>6.1</v>
       </c>
       <c r="B52" s="64" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C52" s="64"/>
-      <c r="D52" s="80" t="s">
-        <v>56</v>
+      <c r="D52" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E52" s="65"/>
       <c r="F52" s="42">
@@ -7993,7 +7602,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K52" s="40"/>
       <c r="L52" s="46"/>
@@ -8053,16 +7662,16 @@
       <c r="BN52" s="46"/>
       <c r="BO52" s="46"/>
     </row>
-    <row r="53" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="53" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="23">
         <v>6.2</v>
       </c>
       <c r="B53" s="64" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C53" s="64"/>
-      <c r="D53" s="80" t="s">
-        <v>56</v>
+      <c r="D53" s="71" t="s">
+        <v>51</v>
       </c>
       <c r="E53" s="65"/>
       <c r="F53" s="42">
@@ -8078,7 +7687,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K53" s="40"/>
       <c r="L53" s="46"/>
@@ -8138,7 +7747,7 @@
       <c r="BN53" s="46"/>
       <c r="BO53" s="46"/>
     </row>
-    <row r="54" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="54" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="23"/>
       <c r="B54" s="64"/>
       <c r="C54" s="64"/>
@@ -8206,7 +7815,7 @@
       <c r="BN54" s="46"/>
       <c r="BO54" s="46"/>
     </row>
-    <row r="55" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="55" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="23"/>
       <c r="B55" s="64"/>
       <c r="C55" s="64"/>
@@ -8274,7 +7883,7 @@
       <c r="BN55" s="46"/>
       <c r="BO55" s="46"/>
     </row>
-    <row r="56" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="56" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="23"/>
       <c r="B56" s="64"/>
       <c r="C56" s="64"/>
@@ -8342,7 +7951,7 @@
       <c r="BN56" s="46"/>
       <c r="BO56" s="46"/>
     </row>
-    <row r="57" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="57" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="23"/>
       <c r="B57" s="64"/>
       <c r="C57" s="64"/>
@@ -8410,7 +8019,7 @@
       <c r="BN57" s="46"/>
       <c r="BO57" s="46"/>
     </row>
-    <row r="58" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="58" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="23"/>
       <c r="C58" s="64"/>
       <c r="E58" s="65"/>
@@ -8477,7 +8086,7 @@
       <c r="BN58" s="46"/>
       <c r="BO58" s="46"/>
     </row>
-    <row r="59" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="59" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="23"/>
       <c r="C59" s="64"/>
       <c r="E59" s="65"/>
@@ -8544,7 +8153,7 @@
       <c r="BN59" s="46"/>
       <c r="BO59" s="46"/>
     </row>
-    <row r="60" spans="1:67" s="24" customFormat="1" ht="18">
+    <row r="60" spans="1:67" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="23"/>
       <c r="C60" s="64"/>
       <c r="E60" s="65"/>
@@ -8614,15 +8223,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -8633,629 +8233,680 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I9 I13 I19:I20 I22:I23 I25:I26 I28 I31:I32 I34 I37:I38 I40 I51:I52 I54 I58 I45:I46">
-    <cfRule type="dataBar" priority="151">
+  <conditionalFormatting sqref="I8:I9 I13 I19:I20 I22:I23 I25 I31:I32 I34 I37:I38 I40 I51:I52 I54 I58 I45:I46">
+    <cfRule type="dataBar" priority="154">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0A58A75E-4698-465A-8593-F06B91A3A900}</x14:id>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B0934F4-049F-459A-8CFB-4EC552EFCB34}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="112" priority="194">
+    <cfRule type="expression" dxfId="100" priority="197">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:BO9 L13:BO17 L19:BO20 L22:BO23">
-    <cfRule type="expression" dxfId="111" priority="197">
+    <cfRule type="expression" dxfId="99" priority="200">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="198">
+    <cfRule type="expression" dxfId="98" priority="201">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO9 L13:BO13 L19:BO20 L22:BO23">
-    <cfRule type="expression" dxfId="109" priority="157">
+    <cfRule type="expression" dxfId="97" priority="160">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="dataBar" priority="146">
+    <cfRule type="dataBar" priority="149">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{DEFF3913-EE89-4EA4-9115-9D21A0823048}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:BO10">
-    <cfRule type="expression" dxfId="108" priority="148">
+    <cfRule type="expression" dxfId="96" priority="151">
       <formula>AND($F10&lt;=L$6,ROUNDDOWN(($G10-$F10+1)*$I10,0)+$F10-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="149">
+    <cfRule type="expression" dxfId="95" priority="152">
       <formula>AND(NOT(ISBLANK($F10)),$F10&lt;=L$6,$G10&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:BO10">
-    <cfRule type="expression" dxfId="106" priority="147">
+    <cfRule type="expression" dxfId="94" priority="150">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="dataBar" priority="142">
+    <cfRule type="dataBar" priority="145">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{815CD2AB-2E6F-403D-80E7-061609C74EF4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:BO11">
-    <cfRule type="expression" dxfId="105" priority="144">
+    <cfRule type="expression" dxfId="93" priority="147">
       <formula>AND($F11&lt;=L$6,ROUNDDOWN(($G11-$F11+1)*$I11,0)+$F11-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="145">
+    <cfRule type="expression" dxfId="92" priority="148">
       <formula>AND(NOT(ISBLANK($F11)),$F11&lt;=L$6,$G11&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:BO11">
-    <cfRule type="expression" dxfId="103" priority="143">
+    <cfRule type="expression" dxfId="91" priority="146">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="dataBar" priority="138">
+    <cfRule type="dataBar" priority="141">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{4DE783D9-BF2C-4E8C-99D9-D83F49490783}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:BO12">
-    <cfRule type="expression" dxfId="102" priority="140">
+    <cfRule type="expression" dxfId="90" priority="143">
       <formula>AND($F12&lt;=L$6,ROUNDDOWN(($G12-$F12+1)*$I12,0)+$F12-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="141">
+    <cfRule type="expression" dxfId="89" priority="144">
       <formula>AND(NOT(ISBLANK($F12)),$F12&lt;=L$6,$G12&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:BO12">
-    <cfRule type="expression" dxfId="100" priority="139">
+    <cfRule type="expression" dxfId="88" priority="142">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="dataBar" priority="134">
+    <cfRule type="dataBar" priority="137">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{FE3BFC5D-DD1E-4E5C-99FD-C5B93745E00E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15:BO15">
-    <cfRule type="expression" dxfId="99" priority="135">
+    <cfRule type="expression" dxfId="87" priority="138">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="dataBar" priority="130">
+    <cfRule type="dataBar" priority="133">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{7EDD0AA6-9198-408E-AC95-B27467D259D6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:BO16">
-    <cfRule type="expression" dxfId="98" priority="131">
+    <cfRule type="expression" dxfId="86" priority="134">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17">
-    <cfRule type="dataBar" priority="126">
+    <cfRule type="dataBar" priority="129">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{F90E373A-CFB8-4601-A0BD-35FE2489FCD0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:BO17">
-    <cfRule type="expression" dxfId="97" priority="127">
+    <cfRule type="expression" dxfId="85" priority="130">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="dataBar" priority="122">
+    <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{EF67816D-6580-40EA-AE8D-F4905457C07F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14:BO14">
-    <cfRule type="expression" dxfId="96" priority="123">
+    <cfRule type="expression" dxfId="84" priority="126">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:BO18">
-    <cfRule type="expression" dxfId="95" priority="120">
+    <cfRule type="expression" dxfId="83" priority="123">
       <formula>AND($F18&lt;=L$6,ROUNDDOWN(($G18-$F18+1)*$I18,0)+$F18-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="121">
+    <cfRule type="expression" dxfId="82" priority="124">
       <formula>AND(NOT(ISBLANK($F18)),$F18&lt;=L$6,$G18&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18">
-    <cfRule type="dataBar" priority="118">
+    <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{9333D35F-E0E5-49C1-A482-B295DBAEAF5A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:BO18">
-    <cfRule type="expression" dxfId="93" priority="119">
+    <cfRule type="expression" dxfId="81" priority="122">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21 I27 I33 I39 I53 I57 I43:I44">
-    <cfRule type="dataBar" priority="114">
+  <conditionalFormatting sqref="I33 I21 I39 I53 I57 I43:I44">
+    <cfRule type="dataBar" priority="117">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{4CB4999D-7F32-4BD0-A21E-79D58F5E0B47}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:BO21">
-    <cfRule type="expression" dxfId="92" priority="116">
+    <cfRule type="expression" dxfId="80" priority="119">
       <formula>AND($F21&lt;=L$6,ROUNDDOWN(($G21-$F21+1)*$I21,0)+$F21-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="117">
+    <cfRule type="expression" dxfId="79" priority="120">
       <formula>AND(NOT(ISBLANK($F21)),$F21&lt;=L$6,$G21&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:BO21">
-    <cfRule type="expression" dxfId="90" priority="115">
+    <cfRule type="expression" dxfId="78" priority="118">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I29:I30 I24 I35:I36 I32 I38 I41:I42 I52 I55:I56 I59:I60 I47:I50">
-    <cfRule type="dataBar" priority="110">
+  <conditionalFormatting sqref="I35:I36 I24 I32 I38 I41:I42 I52 I55:I56 I59:I60 I47:I50 I29:I30">
+    <cfRule type="dataBar" priority="113">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FE0A2372-87F7-425B-944F-6D9C2BCFEFD9}</x14:id>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E6F040FB-8FF3-46BF-AFB8-E322110300CC}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:BO24">
-    <cfRule type="expression" dxfId="89" priority="112">
+    <cfRule type="expression" dxfId="77" priority="115">
       <formula>AND($F24&lt;=L$6,ROUNDDOWN(($G24-$F24+1)*$I24,0)+$F24-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="113">
+    <cfRule type="expression" dxfId="76" priority="116">
       <formula>AND(NOT(ISBLANK($F24)),$F24&lt;=L$6,$G24&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24:BO24">
-    <cfRule type="expression" dxfId="87" priority="111">
+    <cfRule type="expression" dxfId="75" priority="114">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:BO26 L28:BO28">
-    <cfRule type="expression" dxfId="86" priority="107">
+    <cfRule type="expression" dxfId="74" priority="110">
       <formula>AND($F25&lt;=L$6,ROUNDDOWN(($G25-$F25+1)*$I25,0)+$F25-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="108">
+    <cfRule type="expression" dxfId="73" priority="111">
       <formula>AND(NOT(ISBLANK($F25)),$F25&lt;=L$6,$G25&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:BO26 L28:BO28">
-    <cfRule type="expression" dxfId="84" priority="106">
+    <cfRule type="expression" dxfId="72" priority="109">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:BO27">
-    <cfRule type="expression" dxfId="83" priority="103">
+    <cfRule type="expression" dxfId="71" priority="106">
       <formula>AND($F27&lt;=L$6,ROUNDDOWN(($G27-$F27+1)*$I27,0)+$F27-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="104">
+    <cfRule type="expression" dxfId="70" priority="107">
       <formula>AND(NOT(ISBLANK($F27)),$F27&lt;=L$6,$G27&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:BO27">
-    <cfRule type="expression" dxfId="81" priority="102">
+    <cfRule type="expression" dxfId="69" priority="105">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:BO29">
-    <cfRule type="expression" dxfId="80" priority="99">
+    <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND($F29&lt;=L$6,ROUNDDOWN(($G29-$F29+1)*$I29,0)+$F29-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="100">
+    <cfRule type="expression" dxfId="67" priority="103">
       <formula>AND(NOT(ISBLANK($F29)),$F29&lt;=L$6,$G29&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29:BO29">
-    <cfRule type="expression" dxfId="78" priority="98">
+    <cfRule type="expression" dxfId="66" priority="101">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:BO30">
-    <cfRule type="expression" dxfId="77" priority="95">
+    <cfRule type="expression" dxfId="65" priority="98">
       <formula>AND($F30&lt;=L$6,ROUNDDOWN(($G30-$F30+1)*$I30,0)+$F30-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="96">
+    <cfRule type="expression" dxfId="64" priority="99">
       <formula>AND(NOT(ISBLANK($F30)),$F30&lt;=L$6,$G30&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:BO30">
-    <cfRule type="expression" dxfId="75" priority="94">
+    <cfRule type="expression" dxfId="63" priority="97">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31:BO32 L34:BO34">
-    <cfRule type="expression" dxfId="74" priority="91">
+    <cfRule type="expression" dxfId="62" priority="94">
       <formula>AND($F31&lt;=L$6,ROUNDDOWN(($G31-$F31+1)*$I31,0)+$F31-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="92">
+    <cfRule type="expression" dxfId="61" priority="95">
       <formula>AND(NOT(ISBLANK($F31)),$F31&lt;=L$6,$G31&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L31:BO32 L34:BO34">
-    <cfRule type="expression" dxfId="72" priority="90">
+    <cfRule type="expression" dxfId="60" priority="93">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33:BO33">
-    <cfRule type="expression" dxfId="71" priority="87">
+    <cfRule type="expression" dxfId="59" priority="90">
       <formula>AND($F33&lt;=L$6,ROUNDDOWN(($G33-$F33+1)*$I33,0)+$F33-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="88">
+    <cfRule type="expression" dxfId="58" priority="91">
       <formula>AND(NOT(ISBLANK($F33)),$F33&lt;=L$6,$G33&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33:BO33">
-    <cfRule type="expression" dxfId="69" priority="86">
+    <cfRule type="expression" dxfId="57" priority="89">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35:BO35">
-    <cfRule type="expression" dxfId="68" priority="83">
+    <cfRule type="expression" dxfId="56" priority="86">
       <formula>AND($F35&lt;=L$6,ROUNDDOWN(($G35-$F35+1)*$I35,0)+$F35-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="84">
+    <cfRule type="expression" dxfId="55" priority="87">
       <formula>AND(NOT(ISBLANK($F35)),$F35&lt;=L$6,$G35&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35:BO35">
-    <cfRule type="expression" dxfId="66" priority="82">
+    <cfRule type="expression" dxfId="54" priority="85">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36:BO36">
-    <cfRule type="expression" dxfId="65" priority="79">
+    <cfRule type="expression" dxfId="53" priority="82">
       <formula>AND($F36&lt;=L$6,ROUNDDOWN(($G36-$F36+1)*$I36,0)+$F36-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="80">
+    <cfRule type="expression" dxfId="52" priority="83">
       <formula>AND(NOT(ISBLANK($F36)),$F36&lt;=L$6,$G36&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L36:BO36">
-    <cfRule type="expression" dxfId="63" priority="78">
+    <cfRule type="expression" dxfId="51" priority="81">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37:BO38 L40:BO40">
-    <cfRule type="expression" dxfId="62" priority="73">
+    <cfRule type="expression" dxfId="50" priority="76">
       <formula>AND($F37&lt;=L$6,ROUNDDOWN(($G37-$F37+1)*$I37,0)+$F37-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="74">
+    <cfRule type="expression" dxfId="49" priority="77">
       <formula>AND(NOT(ISBLANK($F37)),$F37&lt;=L$6,$G37&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37:BO38 L40:BO40">
-    <cfRule type="expression" dxfId="60" priority="72">
+    <cfRule type="expression" dxfId="48" priority="75">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="59" priority="68">
+    <cfRule type="expression" dxfId="47" priority="71">
       <formula>AND($F39&lt;=L$6,ROUNDDOWN(($G39-$F39+1)*$I39,0)+$F39-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="69">
+    <cfRule type="expression" dxfId="46" priority="72">
       <formula>AND(NOT(ISBLANK($F39)),$F39&lt;=L$6,$G39&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39:BO39">
-    <cfRule type="expression" dxfId="57" priority="67">
+    <cfRule type="expression" dxfId="45" priority="70">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41:BO41">
-    <cfRule type="expression" dxfId="56" priority="64">
+    <cfRule type="expression" dxfId="44" priority="67">
       <formula>AND($F41&lt;=L$6,ROUNDDOWN(($G41-$F41+1)*$I41,0)+$F41-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="65">
+    <cfRule type="expression" dxfId="43" priority="68">
       <formula>AND(NOT(ISBLANK($F41)),$F41&lt;=L$6,$G41&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41:BO41">
-    <cfRule type="expression" dxfId="54" priority="63">
+    <cfRule type="expression" dxfId="42" priority="66">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L42:BO42">
-    <cfRule type="expression" dxfId="53" priority="60">
+    <cfRule type="expression" dxfId="41" priority="63">
       <formula>AND($F42&lt;=L$6,ROUNDDOWN(($G42-$F42+1)*$I42,0)+$F42-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="61">
+    <cfRule type="expression" dxfId="40" priority="64">
       <formula>AND(NOT(ISBLANK($F42)),$F42&lt;=L$6,$G42&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L42:BO42">
-    <cfRule type="expression" dxfId="51" priority="59">
+    <cfRule type="expression" dxfId="39" priority="62">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:BO44">
-    <cfRule type="expression" dxfId="50" priority="55">
+    <cfRule type="expression" dxfId="38" priority="58">
       <formula>AND($F43&lt;=L$6,ROUNDDOWN(($G43-$F43+1)*$I43,0)+$F43-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="56">
+    <cfRule type="expression" dxfId="37" priority="59">
       <formula>AND(NOT(ISBLANK($F43)),$F43&lt;=L$6,$G43&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43:BO44">
-    <cfRule type="expression" dxfId="48" priority="54">
+    <cfRule type="expression" dxfId="36" priority="57">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:BO46">
-    <cfRule type="expression" dxfId="47" priority="51">
+    <cfRule type="expression" dxfId="35" priority="54">
       <formula>AND($F45&lt;=L$6,ROUNDDOWN(($G45-$F45+1)*$I45,0)+$F45-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="52">
+    <cfRule type="expression" dxfId="34" priority="55">
       <formula>AND(NOT(ISBLANK($F45)),$F45&lt;=L$6,$G45&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:BO46">
-    <cfRule type="expression" dxfId="45" priority="50">
+    <cfRule type="expression" dxfId="33" priority="53">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47:BO48">
-    <cfRule type="expression" dxfId="44" priority="47">
+    <cfRule type="expression" dxfId="32" priority="50">
       <formula>AND($F47&lt;=L$6,ROUNDDOWN(($G47-$F47+1)*$I47,0)+$F47-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="48">
+    <cfRule type="expression" dxfId="31" priority="51">
       <formula>AND(NOT(ISBLANK($F47)),$F47&lt;=L$6,$G47&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47:BO48">
-    <cfRule type="expression" dxfId="42" priority="46">
+    <cfRule type="expression" dxfId="30" priority="49">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49:BO50">
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="29" priority="46">
       <formula>AND($F49&lt;=L$6,ROUNDDOWN(($G49-$F49+1)*$I49,0)+$F49-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="44">
+    <cfRule type="expression" dxfId="28" priority="47">
       <formula>AND(NOT(ISBLANK($F49)),$F49&lt;=L$6,$G49&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49:BO50">
-    <cfRule type="expression" dxfId="39" priority="42">
+    <cfRule type="expression" dxfId="27" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51:BO52 L54:BO54">
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="26" priority="41">
       <formula>AND($F51&lt;=L$6,ROUNDDOWN(($G51-$F51+1)*$I51,0)+$F51-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="25" priority="42">
       <formula>AND(NOT(ISBLANK($F51)),$F51&lt;=L$6,$G51&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51:BO52 L54:BO54">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="24" priority="40">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53:BO53">
-    <cfRule type="expression" dxfId="35" priority="33">
+    <cfRule type="expression" dxfId="23" priority="36">
       <formula>AND($F53&lt;=L$6,ROUNDDOWN(($G53-$F53+1)*$I53,0)+$F53-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="34">
+    <cfRule type="expression" dxfId="22" priority="37">
       <formula>AND(NOT(ISBLANK($F53)),$F53&lt;=L$6,$G53&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53:BO53">
-    <cfRule type="expression" dxfId="33" priority="32">
+    <cfRule type="expression" dxfId="21" priority="35">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:BO55">
-    <cfRule type="expression" dxfId="32" priority="29">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>AND($F55&lt;=L$6,ROUNDDOWN(($G55-$F55+1)*$I55,0)+$F55-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="30">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>AND(NOT(ISBLANK($F55)),$F55&lt;=L$6,$G55&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:BO55">
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="18" priority="31">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56:BO56">
-    <cfRule type="expression" dxfId="29" priority="25">
+    <cfRule type="expression" dxfId="17" priority="28">
       <formula>AND($F56&lt;=L$6,ROUNDDOWN(($G56-$F56+1)*$I56,0)+$F56-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="16" priority="29">
       <formula>AND(NOT(ISBLANK($F56)),$F56&lt;=L$6,$G56&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56:BO56">
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="15" priority="27">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:BO57">
-    <cfRule type="expression" dxfId="26" priority="20">
+    <cfRule type="expression" dxfId="14" priority="23">
       <formula>AND($F57&lt;=L$6,ROUNDDOWN(($G57-$F57+1)*$I57,0)+$F57-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="13" priority="24">
       <formula>AND(NOT(ISBLANK($F57)),$F57&lt;=L$6,$G57&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57:BO57">
-    <cfRule type="expression" dxfId="24" priority="19">
+    <cfRule type="expression" dxfId="12" priority="22">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58:BO58">
-    <cfRule type="expression" dxfId="23" priority="16">
+    <cfRule type="expression" dxfId="11" priority="19">
       <formula>AND($F58&lt;=L$6,ROUNDDOWN(($G58-$F58+1)*$I58,0)+$F58-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="17">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>AND(NOT(ISBLANK($F58)),$F58&lt;=L$6,$G58&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58:BO58">
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59:BO59">
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="8" priority="15">
       <formula>AND($F59&lt;=L$6,ROUNDDOWN(($G59-$F59+1)*$I59,0)+$F59-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>AND(NOT(ISBLANK($F59)),$F59&lt;=L$6,$G59&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59:BO59">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:BO60">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>AND($F60&lt;=L$6,ROUNDDOWN(($G60-$F60+1)*$I60,0)+$F60-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="9">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(NOT(ISBLANK($F60)),$F60&lt;=L$6,$G60&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L60:BO60">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{0A58A75E-4698-465A-8593-F06B91A3A900}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color theme="0" tint="-0.34998626667073579"/>
       </dataBar>
-      <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <ext uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{FE0A2372-87F7-425B-944F-6D9C2BCFEFD9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53:BO53">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>AND($F53&lt;=L$6,ROUNDDOWN(($G53-$F53+1)*$I53,0)+$F53-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>AND(NOT(ISBLANK($F53)),$F53&lt;=L$6,$G53&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53:BO53">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I26">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{686FCF22-AD95-49A7-A5F3-A09258557155}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{C60C0BB9-0086-44D9-95A7-243C468A714A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{281B9BEB-E466-41FC-8DCC-90F674CE9544}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -9270,11 +8921,39 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
-  <extLst xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-    <ext uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="8238" r:id="rId4" name="Scroll Bar 46">
+              <controlPr defaultSize="0" print="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>123825</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>28</xdr:col>
+                    <xdr:colOff>104775</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0A58A75E-4698-465A-8593-F06B91A3A900}">
+          <x14:cfRule type="dataBar" id="{5B0934F4-049F-459A-8CFB-4EC552EFCB34}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -9286,7 +8965,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H9 H13 H19:H20 H22:H23</xm:sqref>
+          <xm:sqref>I8:I9 I13 I19:I20 I22:I23 I25 I31:I32 I34 I37:I38 I40 I51:I52 I54 I58 I45:I46</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DEFF3913-EE89-4EA4-9115-9D21A0823048}">
@@ -9301,7 +8980,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H10</xm:sqref>
+          <xm:sqref>I10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{815CD2AB-2E6F-403D-80E7-061609C74EF4}">
@@ -9316,7 +8995,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H11</xm:sqref>
+          <xm:sqref>I11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4DE783D9-BF2C-4E8C-99D9-D83F49490783}">
@@ -9331,7 +9010,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H12</xm:sqref>
+          <xm:sqref>I12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FE3BFC5D-DD1E-4E5C-99FD-C5B93745E00E}">
@@ -9346,7 +9025,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H15</xm:sqref>
+          <xm:sqref>I15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{7EDD0AA6-9198-408E-AC95-B27467D259D6}">
@@ -9361,7 +9040,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H16</xm:sqref>
+          <xm:sqref>I16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F90E373A-CFB8-4601-A0BD-35FE2489FCD0}">
@@ -9376,7 +9055,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H17</xm:sqref>
+          <xm:sqref>I17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{EF67816D-6580-40EA-AE8D-F4905457C07F}">
@@ -9391,7 +9070,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H14</xm:sqref>
+          <xm:sqref>I14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9333D35F-E0E5-49C1-A482-B295DBAEAF5A}">
@@ -9406,7 +9085,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H18</xm:sqref>
+          <xm:sqref>I18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4CB4999D-7F32-4BD0-A21E-79D58F5E0B47}">
@@ -9421,7 +9100,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H21</xm:sqref>
+          <xm:sqref>I33 I21 I39 I53 I57 I43:I44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E6F040FB-8FF3-46BF-AFB8-E322110300CC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I35:I36 I24 I32 I38 I41:I42 I52 I55:I56 I59:I60 I47:I50 I29:I30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0A58A75E-4698-465A-8593-F06B91A3A900}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FE0A2372-87F7-425B-944F-6D9C2BCFEFD9}">
@@ -9436,7 +9145,52 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H24</xm:sqref>
+          <xm:sqref>I53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{686FCF22-AD95-49A7-A5F3-A09258557155}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C60C0BB9-0086-44D9-95A7-243C468A714A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{281B9BEB-E466-41FC-8DCC-90F674CE9544}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>